<commit_message>
updated files for fab
these Gerber's made it to production. the RGB cutout was still wrong, this is the newest rev.
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for Heliotrope_Mini/BOM/Bill of Materials-Heliotrope_Mini.xlsx
+++ b/Hardware/Project Outputs for Heliotrope_Mini/BOM/Bill of Materials-Heliotrope_Mini.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\Heliotrope_Mini\Project Outputs for Heliotrope_Mini\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46D33584-D594-418A-92AC-59B93A614FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{104D6A09-8AD0-4D0A-BFF1-A1E62FE38359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="3660" windowWidth="28800" windowHeight="15435" xr2:uid="{2F3FBF12-13B0-4372-A05D-88E29896650E}"/>
+    <workbookView xWindow="2025" yWindow="3660" windowWidth="28800" windowHeight="15435" xr2:uid="{16A224E9-03EF-4433-B84B-27847F08D38F}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Heliotrope_Mi" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F32B4F6-E039-444A-B6D6-C45F9685E951}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD68008-7F82-4B70-A984-DB5C1D6C50D9}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
updated fab files from altium
created manufacturing zip
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for Heliotrope_Mini/BOM/Bill of Materials-Heliotrope_Mini.xlsx
+++ b/Hardware/Project Outputs for Heliotrope_Mini/BOM/Bill of Materials-Heliotrope_Mini.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\Heliotrope_Mini\Project Outputs for Heliotrope_Mini\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D04A92B-31D5-4B65-9256-7331BDF783ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD22A125-1143-4643-A8CB-57DABC8E7BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="4470" windowWidth="18720" windowHeight="15435" xr2:uid="{83026941-0C40-4609-B27D-22785BC373C6}"/>
+    <workbookView xWindow="13500" yWindow="3495" windowWidth="18720" windowHeight="15435" xr2:uid="{69E9AD88-6833-464E-ABD7-03503AC323DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Heliotrope_Mi" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26991CF9-00AD-41F9-902D-9A6EAA51D88E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E69EB7-3054-494C-9B3A-0E69E6F24E57}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>